<commit_message>
Uploaded 29-Oct-2019 14:16:13 {/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx
+++ b/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t xml:space="preserve">RuleSet</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t xml:space="preserve">com.myspace.pet_rule.RulesParams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
   </si>
   <si>
     <t xml:space="preserve">RuleTable Rules</t>
@@ -409,10 +415,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H41" activeCellId="0" sqref="H41"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -459,411 +465,432 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="F4" s="0"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="F5" s="0"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="0"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="2" t="s">
+      <c r="F7" s="0"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="E10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="F10" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="G10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="H10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="5" t="s">
+    </row>
+    <row r="11" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="E11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="G11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="9" t="n">
+      <c r="H11" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="10" t="n">
+      <c r="C12" s="10" t="n">
         <v>399</v>
       </c>
-      <c r="D9" s="11" t="n">
+      <c r="D12" s="11" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E9" s="12" t="n">
+      <c r="E12" s="12" t="n">
         <v>0.92</v>
       </c>
-      <c r="F9" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="14" t="n">
-        <f aca="false">F9*E9</f>
+      <c r="F12" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="14" t="n">
+        <f aca="false">F12*E12</f>
         <v>0.92</v>
       </c>
-      <c r="H9" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="H12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="0" t="n">
+      <c r="I12" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="14" t="n">
-        <f aca="false">F10*E10</f>
-        <v>1</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="E13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="14" t="n">
+        <f aca="false">F13*E13</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="9" t="n">
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="C11" s="10" t="n">
+      <c r="C14" s="10" t="n">
         <v>400</v>
       </c>
-      <c r="D11" s="11" t="n">
+      <c r="D14" s="11" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E11" s="12" t="n">
+      <c r="E14" s="12" t="n">
         <v>0.92</v>
       </c>
-      <c r="F11" s="13" t="n">
+      <c r="F14" s="13" t="n">
         <v>1.25</v>
       </c>
-      <c r="G11" s="14" t="n">
-        <f aca="false">F11*E11</f>
+      <c r="G14" s="14" t="n">
+        <f aca="false">F14*E14</f>
         <v>1.15</v>
       </c>
-      <c r="H11" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="0" t="n">
+      <c r="H14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="15" t="n">
+      <c r="E15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="15" t="n">
         <v>1.25</v>
       </c>
-      <c r="G12" s="14" t="n">
-        <f aca="false">F12*E12</f>
+      <c r="G15" s="14" t="n">
+        <f aca="false">F15*E15</f>
         <v>1.25</v>
       </c>
-      <c r="H12" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="H15" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="9" t="n">
+      <c r="I15" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="C13" s="10" t="n">
+      <c r="C16" s="10" t="n">
         <v>800</v>
       </c>
-      <c r="D13" s="11" t="n">
+      <c r="D16" s="11" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E13" s="12" t="n">
+      <c r="E16" s="12" t="n">
         <v>0.92</v>
       </c>
-      <c r="F13" s="13" t="n">
+      <c r="F16" s="13" t="n">
         <v>1.5</v>
       </c>
-      <c r="G13" s="14" t="n">
-        <f aca="false">F13*E13</f>
+      <c r="G16" s="14" t="n">
+        <f aca="false">F16*E16</f>
         <v>1.38</v>
       </c>
-      <c r="H13" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="0" t="n">
+      <c r="H16" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" s="15" t="n">
+      <c r="E17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="15" t="n">
         <v>1.5</v>
       </c>
-      <c r="G14" s="14" t="n">
-        <f aca="false">F14*E14</f>
+      <c r="G17" s="14" t="n">
+        <f aca="false">F17*E17</f>
         <v>1.5</v>
       </c>
-      <c r="H14" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="H17" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="9" t="n">
+      <c r="I17" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="C15" s="10" t="n">
+      <c r="C18" s="10" t="n">
         <v>1500</v>
       </c>
-      <c r="D15" s="11" t="n">
+      <c r="D18" s="11" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E15" s="12" t="n">
+      <c r="E18" s="12" t="n">
         <v>0.92</v>
       </c>
-      <c r="F15" s="13" t="n">
+      <c r="F18" s="13" t="n">
         <v>1.75</v>
       </c>
-      <c r="G15" s="14" t="n">
-        <f aca="false">F15*E15</f>
+      <c r="G18" s="14" t="n">
+        <f aca="false">F18*E18</f>
         <v>1.61</v>
       </c>
-      <c r="H15" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="0" t="n">
+      <c r="H18" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" s="15" t="n">
+      <c r="E19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="15" t="n">
         <v>1.75</v>
       </c>
-      <c r="G16" s="14" t="n">
-        <f aca="false">F16*E16</f>
+      <c r="G19" s="14" t="n">
+        <f aca="false">F19*E19</f>
         <v>1.75</v>
       </c>
-      <c r="H16" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="H19" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="9" t="n">
+      <c r="I19" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="C17" s="10" t="n">
+      <c r="C20" s="10" t="n">
         <v>2000</v>
       </c>
-      <c r="D17" s="11" t="n">
+      <c r="D20" s="11" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E17" s="12" t="n">
+      <c r="E20" s="12" t="n">
         <v>0.92</v>
       </c>
-      <c r="F17" s="13" t="n">
+      <c r="F20" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="G17" s="14" t="n">
-        <f aca="false">F17*E17</f>
+      <c r="G20" s="14" t="n">
+        <f aca="false">F20*E20</f>
         <v>1.84</v>
       </c>
-      <c r="H17" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="0" t="n">
+      <c r="H20" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" s="15" t="n">
+      <c r="E21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="G18" s="14" t="n">
-        <f aca="false">F18*E18</f>
+      <c r="G21" s="14" t="n">
+        <f aca="false">F21*E21</f>
         <v>2</v>
       </c>
-      <c r="H18" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="H21" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Uploaded 29-Oct-2019 14:19:31 {/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx
+++ b/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t xml:space="preserve">RuleSet</t>
   </si>
@@ -32,12 +32,6 @@
   </si>
   <si>
     <t xml:space="preserve">com.myspace.pet_rule.RulesParams</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
   </si>
   <si>
     <t xml:space="preserve">RuleTable Rules</t>
@@ -415,10 +409,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -457,440 +451,422 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>4</v>
-      </c>
       <c r="F3" s="0"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="0"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F5" s="0"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="0"/>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F7" s="0"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="A9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="10" t="n">
+        <v>399</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E9" s="12" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="F9" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="14" t="n">
+        <f aca="false">F9*E9</f>
+        <v>0.92</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="7" t="s">
+      <c r="A10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="0" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="14" t="n">
+        <f aca="false">F10*E10</f>
+        <v>1</v>
+      </c>
+      <c r="H10" s="14" t="s">
         <v>26</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="10" t="n">
+        <v>400</v>
+      </c>
+      <c r="D11" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E11" s="12" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="F11" s="13" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G11" s="14" t="n">
+        <f aca="false">F11*E11</f>
+        <v>1.15</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C12" s="10" t="n">
-        <v>399</v>
-      </c>
-      <c r="D12" s="11" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E12" s="12" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="F12" s="13" t="n">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="0" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="15" t="n">
+        <v>1.25</v>
       </c>
       <c r="G12" s="14" t="n">
         <f aca="false">F12*E12</f>
-        <v>0.92</v>
+        <v>1.25</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B13" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" s="10" t="n">
+        <v>800</v>
+      </c>
+      <c r="D13" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="12" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="F13" s="13" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G13" s="14" t="n">
+        <f aca="false">F13*E13</f>
+        <v>1.38</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="14" t="n">
-        <f aca="false">F13*E13</f>
-        <v>1</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="9" t="n">
-        <v>3</v>
-      </c>
-      <c r="C14" s="10" t="n">
-        <v>400</v>
-      </c>
-      <c r="D14" s="11" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E14" s="12" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="F14" s="13" t="n">
-        <v>1.25</v>
+      <c r="E14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="15" t="n">
+        <v>1.5</v>
       </c>
       <c r="G14" s="14" t="n">
         <f aca="false">F14*E14</f>
-        <v>1.15</v>
+        <v>1.5</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B15" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C15" s="10" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D15" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E15" s="12" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="F15" s="13" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="G15" s="14" t="n">
+        <f aca="false">F15*E15</f>
+        <v>1.61</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" s="15" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="G15" s="14" t="n">
-        <f aca="false">F15*E15</f>
-        <v>1.25</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="C16" s="10" t="n">
-        <v>800</v>
-      </c>
-      <c r="D16" s="11" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E16" s="12" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="F16" s="13" t="n">
-        <v>1.5</v>
+      <c r="E16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="15" t="n">
+        <v>1.75</v>
       </c>
       <c r="G16" s="14" t="n">
         <f aca="false">F16*E16</f>
-        <v>1.38</v>
+        <v>1.75</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B17" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C17" s="10" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D17" s="11" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E17" s="12" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="F17" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" s="14" t="n">
+        <f aca="false">F17*E17</f>
+        <v>1.84</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" s="15" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G17" s="14" t="n">
-        <f aca="false">F17*E17</f>
-        <v>1.5</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="C18" s="10" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D18" s="11" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E18" s="12" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="F18" s="13" t="n">
-        <v>1.75</v>
+      <c r="E18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="15" t="n">
+        <v>2</v>
       </c>
       <c r="G18" s="14" t="n">
         <f aca="false">F18*E18</f>
-        <v>1.61</v>
+        <v>2</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="15" t="n">
-        <v>1.75</v>
-      </c>
-      <c r="G19" s="14" t="n">
-        <f aca="false">F19*E19</f>
-        <v>1.75</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="9" t="n">
-        <v>10</v>
-      </c>
-      <c r="C20" s="10" t="n">
-        <v>2000</v>
-      </c>
-      <c r="D20" s="11" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E20" s="12" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="F20" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="G20" s="14" t="n">
-        <f aca="false">F20*E20</f>
-        <v>1.84</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F21" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="G21" s="14" t="n">
-        <f aca="false">F21*E21</f>
-        <v>2</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-    </row>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Uploaded 29-Oct-2019 14:21:14 {/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx
+++ b/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx
@@ -67,10 +67,10 @@
     <t xml:space="preserve">ratingFactor==$param</t>
   </si>
   <si>
-    <t xml:space="preserve">$p.setModifiedRatingFactor($param)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$p.setTier($param)</t>
+    <t xml:space="preserve">$p.setModifiedRatingFactor(“$param”);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$p.setTier(“$param”);</t>
   </si>
   <si>
     <t xml:space="preserve">Rule Name</t>
@@ -412,7 +412,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -423,7 +423,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.9"/>
   </cols>

</xml_diff>

<commit_message>
Uploaded 29-Oct-2019 14:25:28 {/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx
+++ b/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx
@@ -67,10 +67,10 @@
     <t xml:space="preserve">ratingFactor==$param</t>
   </si>
   <si>
-    <t xml:space="preserve">$p.setModifiedRatingFactor(“$param”);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$p.setTier(“$param”);</t>
+    <t xml:space="preserve">$p.setModifiedRatingFactor($param);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$p.setTier($param);</t>
   </si>
   <si>
     <t xml:space="preserve">Rule Name</t>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">Rule 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Tier1</t>
+    <t xml:space="preserve">“Tier1”</t>
   </si>
   <si>
     <t xml:space="preserve">first-hit-policy-group Rules</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Rule 3</t>
   </si>
   <si>
-    <t xml:space="preserve">Tier2</t>
+    <t xml:space="preserve">“Tier2”</t>
   </si>
   <si>
     <t xml:space="preserve">Rule 4</t>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">Rule 5</t>
   </si>
   <si>
-    <t xml:space="preserve">Tier3</t>
+    <t xml:space="preserve">“Tier3”</t>
   </si>
   <si>
     <t xml:space="preserve">Rule 6</t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">Rule 7</t>
   </si>
   <si>
-    <t xml:space="preserve">Tier4</t>
+    <t xml:space="preserve">“Tier4”</t>
   </si>
   <si>
     <t xml:space="preserve">Rule 8</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Rule 9</t>
   </si>
   <si>
-    <t xml:space="preserve">Tier5</t>
+    <t xml:space="preserve">“Tier5”</t>
   </si>
   <si>
     <t xml:space="preserve">Rule 10</t>
@@ -412,7 +412,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Uploaded 29-Oct-2019 14:29:53 {/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx
+++ b/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx
@@ -100,7 +100,7 @@
     <t xml:space="preserve">Rule 1</t>
   </si>
   <si>
-    <t xml:space="preserve">“Tier1”</t>
+    <t xml:space="preserve">"Tier1"</t>
   </si>
   <si>
     <t xml:space="preserve">first-hit-policy-group Rules</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Rule 3</t>
   </si>
   <si>
-    <t xml:space="preserve">“Tier2”</t>
+    <t xml:space="preserve">"Tier2"</t>
   </si>
   <si>
     <t xml:space="preserve">Rule 4</t>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">Rule 5</t>
   </si>
   <si>
-    <t xml:space="preserve">“Tier3”</t>
+    <t xml:space="preserve">"Tier3"</t>
   </si>
   <si>
     <t xml:space="preserve">Rule 6</t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">Rule 7</t>
   </si>
   <si>
-    <t xml:space="preserve">“Tier4”</t>
+    <t xml:space="preserve">"Tier4"</t>
   </si>
   <si>
     <t xml:space="preserve">Rule 8</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Rule 9</t>
   </si>
   <si>
-    <t xml:space="preserve">“Tier5”</t>
+    <t xml:space="preserve">"Tier5"</t>
   </si>
   <si>
     <t xml:space="preserve">Rule 10</t>
@@ -152,7 +152,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -198,6 +198,12 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -259,7 +265,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -321,6 +327,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -412,7 +422,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -603,7 +613,7 @@
         <f aca="false">F10*E10</f>
         <v>1</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="16" t="s">
         <v>26</v>
       </c>
       <c r="I10" s="0" t="s">
@@ -634,7 +644,7 @@
         <f aca="false">F11*E11</f>
         <v>1.15</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="16" t="s">
         <v>30</v>
       </c>
       <c r="I11" s="0" t="s">
@@ -661,7 +671,7 @@
         <f aca="false">F12*E12</f>
         <v>1.25</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="16" t="s">
         <v>30</v>
       </c>
       <c r="I12" s="0" t="s">
@@ -692,7 +702,7 @@
         <f aca="false">F13*E13</f>
         <v>1.38</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="16" t="s">
         <v>33</v>
       </c>
       <c r="I13" s="0" t="s">
@@ -719,7 +729,7 @@
         <f aca="false">F14*E14</f>
         <v>1.5</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="16" t="s">
         <v>33</v>
       </c>
       <c r="I14" s="0" t="s">
@@ -750,7 +760,7 @@
         <f aca="false">F15*E15</f>
         <v>1.61</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="16" t="s">
         <v>36</v>
       </c>
       <c r="I15" s="0" t="s">
@@ -777,7 +787,7 @@
         <f aca="false">F16*E16</f>
         <v>1.75</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="16" t="s">
         <v>36</v>
       </c>
       <c r="I16" s="0" t="s">
@@ -808,7 +818,7 @@
         <f aca="false">F17*E17</f>
         <v>1.84</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="16" t="s">
         <v>39</v>
       </c>
       <c r="I17" s="0" t="s">
@@ -835,7 +845,7 @@
         <f aca="false">F18*E18</f>
         <v>2</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="16" t="s">
         <v>39</v>
       </c>
       <c r="I18" s="0" t="s">
@@ -843,13 +853,13 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Uploaded 29-Oct-2019 14:32:58 {/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx
+++ b/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx
@@ -149,8 +149,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -265,7 +266,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -319,6 +320,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -422,7 +427,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -583,10 +588,9 @@
         <v>1</v>
       </c>
       <c r="G9" s="14" t="n">
-        <f aca="false">F9*E9</f>
         <v>0.92</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="15" t="s">
         <v>26</v>
       </c>
       <c r="I9" s="0" t="s">
@@ -606,14 +610,13 @@
       <c r="E10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F10" s="15" t="n">
+      <c r="F10" s="16" t="n">
         <v>1</v>
       </c>
       <c r="G10" s="14" t="n">
-        <f aca="false">F10*E10</f>
-        <v>1</v>
-      </c>
-      <c r="H10" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="17" t="s">
         <v>26</v>
       </c>
       <c r="I10" s="0" t="s">
@@ -641,10 +644,9 @@
         <v>1.25</v>
       </c>
       <c r="G11" s="14" t="n">
-        <f aca="false">F11*E11</f>
         <v>1.15</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="17" t="s">
         <v>30</v>
       </c>
       <c r="I11" s="0" t="s">
@@ -664,14 +666,13 @@
       <c r="E12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F12" s="15" t="n">
+      <c r="F12" s="16" t="n">
         <v>1.25</v>
       </c>
       <c r="G12" s="14" t="n">
-        <f aca="false">F12*E12</f>
         <v>1.25</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="17" t="s">
         <v>30</v>
       </c>
       <c r="I12" s="0" t="s">
@@ -699,10 +700,9 @@
         <v>1.5</v>
       </c>
       <c r="G13" s="14" t="n">
-        <f aca="false">F13*E13</f>
         <v>1.38</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="17" t="s">
         <v>33</v>
       </c>
       <c r="I13" s="0" t="s">
@@ -722,14 +722,13 @@
       <c r="E14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F14" s="15" t="n">
+      <c r="F14" s="16" t="n">
         <v>1.5</v>
       </c>
       <c r="G14" s="14" t="n">
-        <f aca="false">F14*E14</f>
         <v>1.5</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="17" t="s">
         <v>33</v>
       </c>
       <c r="I14" s="0" t="s">
@@ -757,10 +756,9 @@
         <v>1.75</v>
       </c>
       <c r="G15" s="14" t="n">
-        <f aca="false">F15*E15</f>
         <v>1.61</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="H15" s="17" t="s">
         <v>36</v>
       </c>
       <c r="I15" s="0" t="s">
@@ -780,14 +778,13 @@
       <c r="E16" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F16" s="15" t="n">
+      <c r="F16" s="16" t="n">
         <v>1.75</v>
       </c>
       <c r="G16" s="14" t="n">
-        <f aca="false">F16*E16</f>
         <v>1.75</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="17" t="s">
         <v>36</v>
       </c>
       <c r="I16" s="0" t="s">
@@ -815,10 +812,9 @@
         <v>2</v>
       </c>
       <c r="G17" s="14" t="n">
-        <f aca="false">F17*E17</f>
         <v>1.84</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="H17" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I17" s="0" t="s">
@@ -838,14 +834,13 @@
       <c r="E18" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="15" t="n">
+      <c r="F18" s="16" t="n">
         <v>2</v>
       </c>
       <c r="G18" s="14" t="n">
-        <f aca="false">F18*E18</f>
         <v>2</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H18" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I18" s="0" t="s">
@@ -853,13 +848,13 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Uploaded 29-Oct-2019 14:42:56 {/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx
+++ b/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx
@@ -588,6 +588,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="14" t="n">
+        <f aca="false">E9*F9</f>
         <v>0.92</v>
       </c>
       <c r="H9" s="15" t="s">
@@ -614,6 +615,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="14" t="n">
+        <f aca="false">E10*F10</f>
         <v>1</v>
       </c>
       <c r="H10" s="17" t="s">
@@ -644,6 +646,7 @@
         <v>1.25</v>
       </c>
       <c r="G11" s="14" t="n">
+        <f aca="false">E11*F11</f>
         <v>1.15</v>
       </c>
       <c r="H11" s="17" t="s">
@@ -670,6 +673,7 @@
         <v>1.25</v>
       </c>
       <c r="G12" s="14" t="n">
+        <f aca="false">E12*F12</f>
         <v>1.25</v>
       </c>
       <c r="H12" s="17" t="s">
@@ -700,6 +704,7 @@
         <v>1.5</v>
       </c>
       <c r="G13" s="14" t="n">
+        <f aca="false">E13*F13</f>
         <v>1.38</v>
       </c>
       <c r="H13" s="17" t="s">
@@ -726,6 +731,7 @@
         <v>1.5</v>
       </c>
       <c r="G14" s="14" t="n">
+        <f aca="false">E14*F14</f>
         <v>1.5</v>
       </c>
       <c r="H14" s="17" t="s">
@@ -756,6 +762,7 @@
         <v>1.75</v>
       </c>
       <c r="G15" s="14" t="n">
+        <f aca="false">E15*F15</f>
         <v>1.61</v>
       </c>
       <c r="H15" s="17" t="s">
@@ -782,6 +789,7 @@
         <v>1.75</v>
       </c>
       <c r="G16" s="14" t="n">
+        <f aca="false">E16*F16</f>
         <v>1.75</v>
       </c>
       <c r="H16" s="17" t="s">
@@ -812,6 +820,7 @@
         <v>2</v>
       </c>
       <c r="G17" s="14" t="n">
+        <f aca="false">E17*F17</f>
         <v>1.84</v>
       </c>
       <c r="H17" s="17" t="s">
@@ -838,6 +847,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="14" t="n">
+        <f aca="false">E18*F18</f>
         <v>2</v>
       </c>
       <c r="H18" s="17" t="s">

</xml_diff>

<commit_message>
Uploaded 29-Oct-2019 14:53:54 {/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx
+++ b/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx
@@ -67,7 +67,7 @@
     <t xml:space="preserve">ratingFactor==$param</t>
   </si>
   <si>
-    <t xml:space="preserve">$p.setModifiedRatingFactor($param);</t>
+    <t xml:space="preserve">$p.setModifiedRatingFactor($p.getFactor()*$p.getRatingFactor());</t>
   </si>
   <si>
     <t xml:space="preserve">$p.setTier($param);</t>
@@ -427,7 +427,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -587,10 +587,7 @@
       <c r="F9" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="G9" s="14" t="n">
-        <f aca="false">E9*F9</f>
-        <v>0.92</v>
-      </c>
+      <c r="G9" s="14"/>
       <c r="H9" s="15" t="s">
         <v>26</v>
       </c>
@@ -614,10 +611,7 @@
       <c r="F10" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="G10" s="14" t="n">
-        <f aca="false">E10*F10</f>
-        <v>1</v>
-      </c>
+      <c r="G10" s="14"/>
       <c r="H10" s="17" t="s">
         <v>26</v>
       </c>
@@ -645,10 +639,7 @@
       <c r="F11" s="13" t="n">
         <v>1.25</v>
       </c>
-      <c r="G11" s="14" t="n">
-        <f aca="false">E11*F11</f>
-        <v>1.15</v>
-      </c>
+      <c r="G11" s="14"/>
       <c r="H11" s="17" t="s">
         <v>30</v>
       </c>
@@ -672,10 +663,7 @@
       <c r="F12" s="16" t="n">
         <v>1.25</v>
       </c>
-      <c r="G12" s="14" t="n">
-        <f aca="false">E12*F12</f>
-        <v>1.25</v>
-      </c>
+      <c r="G12" s="14"/>
       <c r="H12" s="17" t="s">
         <v>30</v>
       </c>
@@ -703,10 +691,7 @@
       <c r="F13" s="13" t="n">
         <v>1.5</v>
       </c>
-      <c r="G13" s="14" t="n">
-        <f aca="false">E13*F13</f>
-        <v>1.38</v>
-      </c>
+      <c r="G13" s="14"/>
       <c r="H13" s="17" t="s">
         <v>33</v>
       </c>
@@ -730,10 +715,7 @@
       <c r="F14" s="16" t="n">
         <v>1.5</v>
       </c>
-      <c r="G14" s="14" t="n">
-        <f aca="false">E14*F14</f>
-        <v>1.5</v>
-      </c>
+      <c r="G14" s="14"/>
       <c r="H14" s="17" t="s">
         <v>33</v>
       </c>
@@ -761,10 +743,7 @@
       <c r="F15" s="13" t="n">
         <v>1.75</v>
       </c>
-      <c r="G15" s="14" t="n">
-        <f aca="false">E15*F15</f>
-        <v>1.61</v>
-      </c>
+      <c r="G15" s="14"/>
       <c r="H15" s="17" t="s">
         <v>36</v>
       </c>
@@ -788,10 +767,7 @@
       <c r="F16" s="16" t="n">
         <v>1.75</v>
       </c>
-      <c r="G16" s="14" t="n">
-        <f aca="false">E16*F16</f>
-        <v>1.75</v>
-      </c>
+      <c r="G16" s="14"/>
       <c r="H16" s="17" t="s">
         <v>36</v>
       </c>
@@ -819,10 +795,7 @@
       <c r="F17" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="G17" s="14" t="n">
-        <f aca="false">E17*F17</f>
-        <v>1.84</v>
-      </c>
+      <c r="G17" s="14"/>
       <c r="H17" s="17" t="s">
         <v>39</v>
       </c>
@@ -846,10 +819,7 @@
       <c r="F18" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="G18" s="14" t="n">
-        <f aca="false">E18*F18</f>
-        <v>2</v>
-      </c>
+      <c r="G18" s="14"/>
       <c r="H18" s="17" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Uploaded 29-Oct-2019 14:56:53 {/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx
+++ b/src/main/resources/com/myspace/pet_rule/Pet Rules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t xml:space="preserve">RuleSet</t>
   </si>
@@ -323,7 +323,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -427,7 +427,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
+      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -438,7 +438,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="58.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.9"/>
   </cols>
@@ -587,7 +587,9 @@
       <c r="F9" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="G9" s="14"/>
+      <c r="G9" s="14" t="s">
+        <v>15</v>
+      </c>
       <c r="H9" s="15" t="s">
         <v>26</v>
       </c>
@@ -611,7 +613,9 @@
       <c r="F10" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="G10" s="14"/>
+      <c r="G10" s="14" t="s">
+        <v>15</v>
+      </c>
       <c r="H10" s="17" t="s">
         <v>26</v>
       </c>
@@ -639,7 +643,9 @@
       <c r="F11" s="13" t="n">
         <v>1.25</v>
       </c>
-      <c r="G11" s="14"/>
+      <c r="G11" s="14" t="s">
+        <v>15</v>
+      </c>
       <c r="H11" s="17" t="s">
         <v>30</v>
       </c>
@@ -663,7 +669,9 @@
       <c r="F12" s="16" t="n">
         <v>1.25</v>
       </c>
-      <c r="G12" s="14"/>
+      <c r="G12" s="14" t="s">
+        <v>15</v>
+      </c>
       <c r="H12" s="17" t="s">
         <v>30</v>
       </c>
@@ -691,7 +699,9 @@
       <c r="F13" s="13" t="n">
         <v>1.5</v>
       </c>
-      <c r="G13" s="14"/>
+      <c r="G13" s="14" t="s">
+        <v>15</v>
+      </c>
       <c r="H13" s="17" t="s">
         <v>33</v>
       </c>
@@ -715,7 +725,9 @@
       <c r="F14" s="16" t="n">
         <v>1.5</v>
       </c>
-      <c r="G14" s="14"/>
+      <c r="G14" s="14" t="s">
+        <v>15</v>
+      </c>
       <c r="H14" s="17" t="s">
         <v>33</v>
       </c>
@@ -743,7 +755,9 @@
       <c r="F15" s="13" t="n">
         <v>1.75</v>
       </c>
-      <c r="G15" s="14"/>
+      <c r="G15" s="14" t="s">
+        <v>15</v>
+      </c>
       <c r="H15" s="17" t="s">
         <v>36</v>
       </c>
@@ -767,7 +781,9 @@
       <c r="F16" s="16" t="n">
         <v>1.75</v>
       </c>
-      <c r="G16" s="14"/>
+      <c r="G16" s="14" t="s">
+        <v>15</v>
+      </c>
       <c r="H16" s="17" t="s">
         <v>36</v>
       </c>
@@ -795,7 +811,9 @@
       <c r="F17" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="G17" s="14"/>
+      <c r="G17" s="14" t="s">
+        <v>15</v>
+      </c>
       <c r="H17" s="17" t="s">
         <v>39</v>
       </c>
@@ -819,7 +837,9 @@
       <c r="F18" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="G18" s="14"/>
+      <c r="G18" s="14" t="s">
+        <v>15</v>
+      </c>
       <c r="H18" s="17" t="s">
         <v>39</v>
       </c>

</xml_diff>